<commit_message>
Aplicado e integrado preguntas y ponderadores
</commit_message>
<xml_diff>
--- a/data/Encuesta.xlsx
+++ b/data/Encuesta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juank\turismo-religioso-analisis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B0F687-FCD6-49EE-8CF6-7AFD63BDAB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE16A585-C34A-4EE8-B871-DD5A34EAC6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12922" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12922" uniqueCount="1121">
   <si>
     <t>ObjectID</t>
   </si>
@@ -3397,6 +3397,9 @@
   </si>
   <si>
     <t>¿Cuál fue el motivo de su viaje a esta ciudad o municipio?</t>
+  </si>
+  <si>
+    <t>¿Cuántos días estará en la ciudad donde se desarrolla este evento</t>
   </si>
 </sst>
 </file>
@@ -3771,7 +3774,7 @@
   <dimension ref="A1:BB580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3841,7 +3844,7 @@
         <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>20</v>
+        <v>1120</v>
       </c>
       <c r="V1" t="s">
         <v>21</v>

</xml_diff>